<commit_message>
Updated Room test spreadsheet with more cases
</commit_message>
<xml_diff>
--- a/test-files/Room Information (Responses).xlsx
+++ b/test-files/Room Information (Responses).xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\workspace\523-Music-Scheduler\test-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Timestamp</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>6:20-7:00 PM, 7:00-7:40 PM</t>
+  </si>
+  <si>
+    <t>Something, Else</t>
+  </si>
+  <si>
+    <t>5:00-5:40 PM</t>
+  </si>
+  <si>
+    <t>Some 123.1</t>
   </si>
 </sst>
 </file>
@@ -404,11 +413,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:G4"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -499,7 +508,7 @@
       <c r="A4" s="1">
         <v>42070.599336550928</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -512,6 +521,29 @@
         <v>16</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>42070.599336550928</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>